<commit_message>
added file with correct BI values
</commit_message>
<xml_diff>
--- a/input/Assessments_JK_V1.2.xlsx
+++ b/input/Assessments_JK_V1.2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arefk\Desktop\Projects\2025_Klein_Behaviour\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliaklein/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3F3F0B-7609-4D4E-A617-B2A381903EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C876DA-D8FD-5E45-84B3-4F8275D7E062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A5EABDC9-F485-304B-BF04-2A0DB9F92F8C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{A5EABDC9-F485-304B-BF04-2A0DB9F92F8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -59,6 +59,9 @@
     <t>BI_T0</t>
   </si>
   <si>
+    <t>mrs_T0</t>
+  </si>
+  <si>
     <t>NIHSS_T0</t>
   </si>
   <si>
@@ -81,9 +84,6 @@
   </si>
   <si>
     <t>record_id</t>
-  </si>
-  <si>
-    <t>MRS_T0</t>
   </si>
 </sst>
 </file>
@@ -130,7 +130,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -146,7 +146,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -464,28 +464,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC453578-E856-074F-80E0-084951BA72A1}">
   <dimension ref="A1:K335"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
+      <selection activeCell="I186" sqref="I186"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.375" customWidth="1"/>
-    <col min="2" max="2" width="20.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="36" customWidth="1"/>
     <col min="10" max="10" width="25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -494,31 +494,31 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -535,7 +535,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -552,7 +552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -560,7 +560,7 @@
         <v>3</v>
       </c>
       <c r="I4">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -569,7 +569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -586,7 +586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -603,7 +603,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -611,7 +611,7 @@
         <v>3</v>
       </c>
       <c r="I7">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="J7">
         <v>2</v>
@@ -620,7 +620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
@@ -637,7 +637,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>4</v>
       </c>
@@ -654,7 +654,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>4</v>
       </c>
@@ -662,7 +662,7 @@
         <v>3</v>
       </c>
       <c r="I10">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="J10">
         <v>2</v>
@@ -671,7 +671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>5</v>
       </c>
@@ -688,12 +688,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>6</v>
       </c>
@@ -710,7 +710,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>6</v>
       </c>
@@ -718,7 +718,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>7</v>
       </c>
@@ -735,7 +735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>7</v>
       </c>
@@ -743,7 +743,7 @@
         <v>3</v>
       </c>
       <c r="I16">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="J16">
         <v>1</v>
@@ -752,7 +752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>8</v>
       </c>
@@ -769,7 +769,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>8</v>
       </c>
@@ -786,7 +786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>8</v>
       </c>
@@ -794,7 +794,7 @@
         <v>3</v>
       </c>
       <c r="I19">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="J19">
         <v>1</v>
@@ -803,7 +803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>9</v>
       </c>
@@ -820,7 +820,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>9</v>
       </c>
@@ -837,7 +837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>9</v>
       </c>
@@ -845,7 +845,7 @@
         <v>3</v>
       </c>
       <c r="I22">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="J22">
         <v>2</v>
@@ -854,7 +854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>10</v>
       </c>
@@ -871,7 +871,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>10</v>
       </c>
@@ -888,7 +888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>10</v>
       </c>
@@ -896,7 +896,7 @@
         <v>3</v>
       </c>
       <c r="I25">
-        <v>3</v>
+        <v>90</v>
       </c>
       <c r="J25">
         <v>2</v>
@@ -905,7 +905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>11</v>
       </c>
@@ -922,7 +922,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>11</v>
       </c>
@@ -930,7 +930,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>12</v>
       </c>
@@ -947,7 +947,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>12</v>
       </c>
@@ -964,7 +964,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>12</v>
       </c>
@@ -972,7 +972,7 @@
         <v>3</v>
       </c>
       <c r="I30">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="J30">
         <v>3</v>
@@ -981,7 +981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>13</v>
       </c>
@@ -998,12 +998,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>14</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>14</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>14</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>3</v>
       </c>
       <c r="I35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J35">
         <v>5</v>
@@ -1054,7 +1054,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>15</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>15</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>15</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>3</v>
       </c>
       <c r="I38">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="J38">
         <v>5</v>
@@ -1105,7 +1105,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>16</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>16</v>
       </c>
@@ -1139,12 +1139,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>17</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>17</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>17</v>
       </c>
@@ -1186,13 +1186,13 @@
         <v>3</v>
       </c>
       <c r="I44">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="J44">
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>18</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>18</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>18</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>3</v>
       </c>
       <c r="I47">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="J47">
         <v>2</v>
@@ -1243,7 +1243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>19</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>19</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>3</v>
       </c>
       <c r="I49">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="J49">
         <v>4</v>
@@ -1277,7 +1277,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>20</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>20</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>3</v>
       </c>
       <c r="I51">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="J51">
         <v>3</v>
@@ -1311,7 +1311,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>21</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>21</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>21</v>
       </c>
@@ -1353,13 +1353,13 @@
         <v>3</v>
       </c>
       <c r="I54">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="J54">
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>22</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>22</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>22</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>3</v>
       </c>
       <c r="I57">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="J57">
         <v>2</v>
@@ -1410,7 +1410,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>23</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>23</v>
       </c>
@@ -1444,12 +1444,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>23</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>24</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>24</v>
       </c>
@@ -1483,12 +1483,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>25</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>25</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>25</v>
       </c>
@@ -1530,13 +1530,13 @@
         <v>3</v>
       </c>
       <c r="I66">
-        <v>3</v>
+        <v>65</v>
       </c>
       <c r="J66">
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>26</v>
       </c>
@@ -1550,12 +1550,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>26</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>27</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>27</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>27</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>28</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>28</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>28</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>3</v>
       </c>
       <c r="I74">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="J74">
         <v>1</v>
@@ -1648,7 +1648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>29</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>29</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>29</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>30</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>30</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>31</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>31</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>31</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>3</v>
       </c>
       <c r="I82">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="J82">
         <v>2</v>
@@ -1766,7 +1766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>32</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>32</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>32</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>33</v>
       </c>
@@ -1825,12 +1825,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>33</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>33</v>
       </c>
@@ -1838,13 +1838,13 @@
         <v>3</v>
       </c>
       <c r="I88">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="J88">
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>34</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>34</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>34</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>3</v>
       </c>
       <c r="I91">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="J91">
         <v>2</v>
@@ -1895,7 +1895,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>35</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>35</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>35</v>
       </c>
@@ -1937,13 +1937,13 @@
         <v>3</v>
       </c>
       <c r="I94">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="J94">
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>36</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>36</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>36</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>3</v>
       </c>
       <c r="I97">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="J97">
         <v>2</v>
@@ -1994,7 +1994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>37</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>37</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>38</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>38</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>38</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>39</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>39</v>
       </c>
@@ -2098,12 +2098,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>39</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>40</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>40</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>40</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>3</v>
       </c>
       <c r="I108">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="J108">
         <v>1</v>
@@ -2154,7 +2154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>41</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>41</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>41</v>
       </c>
@@ -2196,7 +2196,7 @@
         <v>3</v>
       </c>
       <c r="I111">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J111">
         <v>5</v>
@@ -2205,7 +2205,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>42</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>42</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>42</v>
       </c>
@@ -2247,7 +2247,7 @@
         <v>3</v>
       </c>
       <c r="I114">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="J114">
         <v>2</v>
@@ -2256,7 +2256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>43</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>43</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>43</v>
       </c>
@@ -2301,7 +2301,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>44</v>
       </c>
@@ -2318,7 +2318,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>44</v>
       </c>
@@ -2335,12 +2335,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>44</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>45</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>45</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>45</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>3</v>
       </c>
       <c r="I123">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="J123">
         <v>2</v>
@@ -2391,7 +2391,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>46</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>46</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>46</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>47</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>47</v>
       </c>
@@ -2467,7 +2467,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>47</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>3</v>
       </c>
       <c r="I129">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="J129">
         <v>1</v>
@@ -2484,7 +2484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>48</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>48</v>
       </c>
@@ -2518,12 +2518,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>48</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>49</v>
       </c>
@@ -2540,7 +2540,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>49</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>49</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>3</v>
       </c>
       <c r="I135">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="J135">
         <v>3</v>
@@ -2574,7 +2574,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>50</v>
       </c>
@@ -2591,7 +2591,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>50</v>
       </c>
@@ -2608,12 +2608,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>50</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>51</v>
       </c>
@@ -2630,7 +2630,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>51</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>51</v>
       </c>
@@ -2655,13 +2655,13 @@
         <v>3</v>
       </c>
       <c r="I141">
-        <v>3</v>
+        <v>80</v>
       </c>
       <c r="J141">
         <v>3</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>52</v>
       </c>
@@ -2678,7 +2678,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>52</v>
       </c>
@@ -2686,7 +2686,7 @@
         <v>5</v>
       </c>
       <c r="I143">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="J143">
         <v>4</v>
@@ -2695,7 +2695,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>53</v>
       </c>
@@ -2712,7 +2712,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>53</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>53</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>3</v>
       </c>
       <c r="I146">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="J146">
         <v>3</v>
@@ -2746,7 +2746,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>54</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>54</v>
       </c>
@@ -2780,12 +2780,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>54</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>55</v>
       </c>
@@ -2802,7 +2802,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>55</v>
       </c>
@@ -2819,7 +2819,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>55</v>
       </c>
@@ -2827,7 +2827,7 @@
         <v>3</v>
       </c>
       <c r="I152">
-        <v>3</v>
+        <v>80</v>
       </c>
       <c r="J152">
         <v>2</v>
@@ -2836,7 +2836,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>56</v>
       </c>
@@ -2853,7 +2853,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>56</v>
       </c>
@@ -2870,7 +2870,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>56</v>
       </c>
@@ -2878,7 +2878,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>57</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>57</v>
       </c>
@@ -2912,12 +2912,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>57</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>58</v>
       </c>
@@ -2934,7 +2934,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>58</v>
       </c>
@@ -2951,7 +2951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>58</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>3</v>
       </c>
       <c r="I161">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="J161">
         <v>1</v>
@@ -2968,7 +2968,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>59</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>59</v>
       </c>
@@ -3002,7 +3002,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>59</v>
       </c>
@@ -3010,7 +3010,7 @@
         <v>3</v>
       </c>
       <c r="I164">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="J164">
         <v>1</v>
@@ -3019,7 +3019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>60</v>
       </c>
@@ -3036,7 +3036,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>60</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>60</v>
       </c>
@@ -3061,13 +3061,13 @@
         <v>3</v>
       </c>
       <c r="I167">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J167">
         <v>5</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>61</v>
       </c>
@@ -3084,7 +3084,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>61</v>
       </c>
@@ -3092,13 +3092,13 @@
         <v>5</v>
       </c>
       <c r="I169">
-        <v>3</v>
+        <v>70</v>
       </c>
       <c r="J169">
         <v>3</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>62</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>62</v>
       </c>
@@ -3132,7 +3132,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>62</v>
       </c>
@@ -3140,7 +3140,7 @@
         <v>3</v>
       </c>
       <c r="I172">
-        <v>2</v>
+        <v>85</v>
       </c>
       <c r="J172">
         <v>3</v>
@@ -3149,7 +3149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>63</v>
       </c>
@@ -3166,7 +3166,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>63</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>63</v>
       </c>
@@ -3191,7 +3191,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>64</v>
       </c>
@@ -3208,7 +3208,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>64</v>
       </c>
@@ -3225,7 +3225,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>64</v>
       </c>
@@ -3233,7 +3233,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>65</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>65</v>
       </c>
@@ -3267,7 +3267,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>65</v>
       </c>
@@ -3275,7 +3275,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>66</v>
       </c>
@@ -3292,7 +3292,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>66</v>
       </c>
@@ -3309,7 +3309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>66</v>
       </c>
@@ -3317,7 +3317,7 @@
         <v>3</v>
       </c>
       <c r="I184">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="J184">
         <v>2</v>
@@ -3326,7 +3326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>67</v>
       </c>
@@ -3343,7 +3343,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>67</v>
       </c>
@@ -3351,13 +3351,13 @@
         <v>5</v>
       </c>
       <c r="I186">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="J186">
         <v>3</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>68</v>
       </c>
@@ -3374,7 +3374,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>68</v>
       </c>
@@ -3391,7 +3391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>68</v>
       </c>
@@ -3399,13 +3399,13 @@
         <v>3</v>
       </c>
       <c r="I189">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="J189">
         <v>2</v>
       </c>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>69</v>
       </c>
@@ -3422,7 +3422,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>69</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>69</v>
       </c>
@@ -3447,7 +3447,7 @@
         <v>3</v>
       </c>
       <c r="I192">
-        <v>3</v>
+        <v>75</v>
       </c>
       <c r="J192">
         <v>3</v>
@@ -3456,7 +3456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>70</v>
       </c>
@@ -3473,7 +3473,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>70</v>
       </c>
@@ -3481,12 +3481,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>70</v>
       </c>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>71</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>71</v>
       </c>
@@ -3511,7 +3511,7 @@
         <v>3</v>
       </c>
       <c r="I197">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="J197">
         <v>1</v>
@@ -3520,7 +3520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>72</v>
       </c>
@@ -3537,7 +3537,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>72</v>
       </c>
@@ -3554,7 +3554,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>72</v>
       </c>
@@ -3562,7 +3562,7 @@
         <v>3</v>
       </c>
       <c r="I200">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="J200">
         <v>4</v>
@@ -3571,7 +3571,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>73</v>
       </c>
@@ -3588,7 +3588,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>73</v>
       </c>
@@ -3605,7 +3605,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>73</v>
       </c>
@@ -3613,7 +3613,7 @@
         <v>3</v>
       </c>
       <c r="I203">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="J203">
         <v>4</v>
@@ -3622,7 +3622,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>74</v>
       </c>
@@ -3639,7 +3639,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>74</v>
       </c>
@@ -3656,12 +3656,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>74</v>
       </c>
     </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>75</v>
       </c>
@@ -3678,7 +3678,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>75</v>
       </c>
@@ -3686,7 +3686,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>76</v>
       </c>
@@ -3703,7 +3703,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>76</v>
       </c>
@@ -3720,7 +3720,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>77</v>
       </c>
@@ -3737,7 +3737,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>77</v>
       </c>
@@ -3754,12 +3754,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>77</v>
       </c>
     </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>78</v>
       </c>
@@ -3776,7 +3776,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>78</v>
       </c>
@@ -3793,7 +3793,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>78</v>
       </c>
@@ -3801,7 +3801,7 @@
         <v>3</v>
       </c>
       <c r="I216">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="J216">
         <v>3</v>
@@ -3810,7 +3810,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>79</v>
       </c>
@@ -3827,7 +3827,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>79</v>
       </c>
@@ -3844,7 +3844,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>79</v>
       </c>
@@ -3852,7 +3852,7 @@
         <v>3</v>
       </c>
       <c r="I219">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="J219">
         <v>3</v>
@@ -3861,7 +3861,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>80</v>
       </c>
@@ -3878,7 +3878,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>80</v>
       </c>
@@ -3895,7 +3895,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>80</v>
       </c>
@@ -3903,7 +3903,7 @@
         <v>3</v>
       </c>
       <c r="I222">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="J222">
         <v>2</v>
@@ -3912,7 +3912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>81</v>
       </c>
@@ -3929,7 +3929,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>81</v>
       </c>
@@ -3946,7 +3946,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>81</v>
       </c>
@@ -3954,7 +3954,7 @@
         <v>3</v>
       </c>
       <c r="I225">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="J225">
         <v>3</v>
@@ -3963,7 +3963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>82</v>
       </c>
@@ -3980,7 +3980,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>82</v>
       </c>
@@ -3997,7 +3997,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>82</v>
       </c>
@@ -4005,7 +4005,7 @@
         <v>3</v>
       </c>
       <c r="I228">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="J228">
         <v>2</v>
@@ -4014,7 +4014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>83</v>
       </c>
@@ -4031,17 +4031,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>83</v>
       </c>
     </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>83</v>
       </c>
     </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>84</v>
       </c>
@@ -4058,7 +4058,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>84</v>
       </c>
@@ -4075,12 +4075,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>84</v>
       </c>
     </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>85</v>
       </c>
@@ -4097,7 +4097,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>85</v>
       </c>
@@ -4114,7 +4114,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>85</v>
       </c>
@@ -4122,7 +4122,7 @@
         <v>3</v>
       </c>
       <c r="I237">
-        <v>3</v>
+        <v>70</v>
       </c>
       <c r="J237">
         <v>3</v>
@@ -4131,7 +4131,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>86</v>
       </c>
@@ -4148,7 +4148,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>86</v>
       </c>
@@ -4165,7 +4165,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>86</v>
       </c>
@@ -4173,7 +4173,7 @@
         <v>3</v>
       </c>
       <c r="I240">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="J240">
         <v>1</v>
@@ -4182,7 +4182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>87</v>
       </c>
@@ -4199,7 +4199,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>87</v>
       </c>
@@ -4216,7 +4216,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>87</v>
       </c>
@@ -4224,13 +4224,13 @@
         <v>3</v>
       </c>
       <c r="I243">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="J243">
         <v>4</v>
       </c>
     </row>
-    <row r="244" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>88</v>
       </c>
@@ -4247,7 +4247,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="245" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>88</v>
       </c>
@@ -4264,7 +4264,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A246">
         <v>88</v>
       </c>
@@ -4272,7 +4272,7 @@
         <v>3</v>
       </c>
       <c r="I246">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="J246">
         <v>3</v>
@@ -4281,7 +4281,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="247" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>89</v>
       </c>
@@ -4298,7 +4298,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A248">
         <v>89</v>
       </c>
@@ -4315,7 +4315,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="249" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A249">
         <v>89</v>
       </c>
@@ -4323,13 +4323,13 @@
         <v>3</v>
       </c>
       <c r="I249">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="J249">
         <v>5</v>
       </c>
     </row>
-    <row r="250" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A250">
         <v>90</v>
       </c>
@@ -4346,7 +4346,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A251">
         <v>90</v>
       </c>
@@ -4363,12 +4363,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="252" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A252">
         <v>90</v>
       </c>
     </row>
-    <row r="253" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A253">
         <v>91</v>
       </c>
@@ -4385,12 +4385,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="254" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>91</v>
       </c>
     </row>
-    <row r="255" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A255">
         <v>92</v>
       </c>
@@ -4407,7 +4407,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="256" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A256">
         <v>92</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="257" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A257">
         <v>92</v>
       </c>
@@ -4432,7 +4432,7 @@
         <v>3</v>
       </c>
       <c r="I257">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="J257">
         <v>2</v>
@@ -4441,7 +4441,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="258" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A258">
         <v>93</v>
       </c>
@@ -4458,7 +4458,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="259" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A259">
         <v>93</v>
       </c>
@@ -4475,7 +4475,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="260" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A260">
         <v>94</v>
       </c>
@@ -4492,7 +4492,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="261" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A261">
         <v>94</v>
       </c>
@@ -4509,7 +4509,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="262" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A262">
         <v>94</v>
       </c>
@@ -4517,13 +4517,13 @@
         <v>3</v>
       </c>
       <c r="I262">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="J262">
         <v>4</v>
       </c>
     </row>
-    <row r="263" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A263">
         <v>95</v>
       </c>
@@ -4540,7 +4540,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="264" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A264">
         <v>95</v>
       </c>
@@ -4557,16 +4557,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="265" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A265">
         <v>95</v>
       </c>
       <c r="B265" t="s">
         <v>3</v>
       </c>
-      <c r="I265">
-        <v>2</v>
-      </c>
       <c r="J265">
         <v>4</v>
       </c>
@@ -4574,7 +4571,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="266" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A266">
         <v>96</v>
       </c>
@@ -4591,7 +4588,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="267" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A267">
         <v>96</v>
       </c>
@@ -4599,7 +4596,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="268" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A268">
         <v>97</v>
       </c>
@@ -4616,7 +4613,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="269" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A269">
         <v>97</v>
       </c>
@@ -4633,12 +4630,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="270" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A270">
         <v>97</v>
       </c>
     </row>
-    <row r="271" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A271">
         <v>98</v>
       </c>
@@ -4655,7 +4652,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="272" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A272">
         <v>98</v>
       </c>
@@ -4672,7 +4669,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A273">
         <v>98</v>
       </c>
@@ -4686,7 +4683,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A274">
         <v>99</v>
       </c>
@@ -4703,7 +4700,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A275">
         <v>99</v>
       </c>
@@ -4720,7 +4717,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A276">
         <v>100</v>
       </c>
@@ -4737,16 +4734,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A277">
         <v>100</v>
       </c>
       <c r="B277" t="s">
         <v>3</v>
       </c>
-      <c r="I277">
-        <v>3</v>
-      </c>
       <c r="J277">
         <v>1</v>
       </c>
@@ -4754,7 +4748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A278">
         <v>101</v>
       </c>
@@ -4771,12 +4765,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A279">
         <v>101</v>
       </c>
     </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A280">
         <v>101</v>
       </c>
@@ -4787,7 +4781,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="281" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A281">
         <v>102</v>
       </c>
@@ -4804,12 +4798,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A282">
         <v>102</v>
       </c>
     </row>
-    <row r="283" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A283">
         <v>103</v>
       </c>
@@ -4826,12 +4820,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="284" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A284">
         <v>103</v>
       </c>
     </row>
-    <row r="285" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A285">
         <v>104</v>
       </c>
@@ -4848,16 +4842,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="286" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A286">
         <v>104</v>
       </c>
       <c r="B286" t="s">
         <v>3</v>
       </c>
-      <c r="I286">
-        <v>3</v>
-      </c>
       <c r="J286">
         <v>3</v>
       </c>
@@ -4865,7 +4856,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="287" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A287">
         <v>105</v>
       </c>
@@ -4882,7 +4873,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="288" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A288">
         <v>105</v>
       </c>
@@ -4899,7 +4890,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A289">
         <v>106</v>
       </c>
@@ -4916,12 +4907,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A290">
         <v>106</v>
       </c>
     </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A291">
         <v>107</v>
       </c>
@@ -4938,7 +4929,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A292">
         <v>107</v>
       </c>
@@ -4955,7 +4946,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A293">
         <v>108</v>
       </c>
@@ -4972,17 +4963,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A294">
         <v>109</v>
       </c>
     </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A295">
         <v>109</v>
       </c>
     </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A296">
         <v>110</v>
       </c>
@@ -4999,12 +4990,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A297">
         <v>110</v>
       </c>
     </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A298">
         <v>111</v>
       </c>
@@ -5021,7 +5012,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A299">
         <v>112</v>
       </c>
@@ -5038,7 +5029,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A300">
         <v>112</v>
       </c>
@@ -5055,7 +5046,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A301">
         <v>112</v>
       </c>
@@ -5063,7 +5054,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A302">
         <v>113</v>
       </c>
@@ -5080,7 +5071,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A303">
         <v>113</v>
       </c>
@@ -5097,7 +5088,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A304">
         <v>113</v>
       </c>
@@ -5111,7 +5102,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="305" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A305">
         <v>114</v>
       </c>
@@ -5128,7 +5119,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="306" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A306">
         <v>114</v>
       </c>
@@ -5145,7 +5136,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="307" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A307">
         <v>115</v>
       </c>
@@ -5162,7 +5153,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="308" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A308">
         <v>115</v>
       </c>
@@ -5179,7 +5170,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="309" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A309">
         <v>116</v>
       </c>
@@ -5196,7 +5187,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="310" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A310">
         <v>116</v>
       </c>
@@ -5213,7 +5204,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="311" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A311">
         <v>117</v>
       </c>
@@ -5230,7 +5221,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="312" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A312">
         <v>117</v>
       </c>
@@ -5247,17 +5238,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A313">
         <v>118</v>
       </c>
     </row>
-    <row r="314" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A314">
         <v>118</v>
       </c>
     </row>
-    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A315">
         <v>119</v>
       </c>
@@ -5274,12 +5265,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="316" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A316">
         <v>119</v>
       </c>
     </row>
-    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A317">
         <v>120</v>
       </c>
@@ -5296,17 +5287,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A318">
         <v>120</v>
       </c>
     </row>
-    <row r="319" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A319">
         <v>121</v>
       </c>
     </row>
-    <row r="320" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A320">
         <v>121</v>
       </c>
@@ -5323,7 +5314,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="321" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A321">
         <v>122</v>
       </c>
@@ -5340,7 +5331,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="322" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A322">
         <v>122</v>
       </c>
@@ -5357,7 +5348,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="323" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A323">
         <v>123</v>
       </c>
@@ -5374,52 +5365,52 @@
         <v>12</v>
       </c>
     </row>
-    <row r="324" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A324">
         <v>123</v>
       </c>
     </row>
-    <row r="325" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A325">
         <v>124</v>
       </c>
     </row>
-    <row r="326" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A326">
         <v>124</v>
       </c>
     </row>
-    <row r="327" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A327">
         <v>125</v>
       </c>
     </row>
-    <row r="328" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A328">
         <v>125</v>
       </c>
     </row>
-    <row r="329" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A329">
         <v>126</v>
       </c>
     </row>
-    <row r="330" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A330">
         <v>126</v>
       </c>
     </row>
-    <row r="331" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A331">
         <v>127</v>
       </c>
     </row>
-    <row r="332" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A332">
         <v>127</v>
       </c>
     </row>
-    <row r="333" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A333">
         <v>128</v>
       </c>
@@ -5436,12 +5427,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="334" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A334">
         <v>129</v>
       </c>
     </row>
-    <row r="335" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A335">
         <v>129</v>
       </c>

</xml_diff>

<commit_message>
added some figures and code about the sanky plot and heatplot, but both need to be adjusted
</commit_message>
<xml_diff>
--- a/input/Assessments_JK_V1.2.xlsx
+++ b/input/Assessments_JK_V1.2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliaklein/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arefk\Desktop\Projects\2025_Klein_Behaviour\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C876DA-D8FD-5E45-84B3-4F8275D7E062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0668CB66-B8E3-439E-95D6-DA5CF4636734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{A5EABDC9-F485-304B-BF04-2A0DB9F92F8C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A5EABDC9-F485-304B-BF04-2A0DB9F92F8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -59,9 +59,6 @@
     <t>BI_T0</t>
   </si>
   <si>
-    <t>mrs_T0</t>
-  </si>
-  <si>
     <t>NIHSS_T0</t>
   </si>
   <si>
@@ -84,6 +81,9 @@
   </si>
   <si>
     <t>record_id</t>
+  </si>
+  <si>
+    <t>MRS_T0</t>
   </si>
 </sst>
 </file>
@@ -130,7 +130,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -146,7 +146,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -464,28 +464,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC453578-E856-074F-80E0-084951BA72A1}">
   <dimension ref="A1:K335"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
-      <selection activeCell="I186" sqref="I186"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.375" customWidth="1"/>
+    <col min="2" max="2" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="36" customWidth="1"/>
     <col min="10" max="10" width="25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -494,31 +494,31 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
       <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -535,7 +535,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -552,7 +552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -569,7 +569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -586,7 +586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -603,7 +603,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -620,7 +620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -637,7 +637,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -654,7 +654,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -671,7 +671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
@@ -688,12 +688,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6</v>
       </c>
@@ -710,7 +710,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6</v>
       </c>
@@ -718,7 +718,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>7</v>
       </c>
@@ -735,7 +735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>7</v>
       </c>
@@ -752,7 +752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>8</v>
       </c>
@@ -769,7 +769,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>8</v>
       </c>
@@ -786,7 +786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>8</v>
       </c>
@@ -803,7 +803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>9</v>
       </c>
@@ -820,7 +820,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>9</v>
       </c>
@@ -837,7 +837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>9</v>
       </c>
@@ -854,7 +854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>10</v>
       </c>
@@ -871,7 +871,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>10</v>
       </c>
@@ -888,7 +888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>10</v>
       </c>
@@ -905,7 +905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>11</v>
       </c>
@@ -922,7 +922,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>11</v>
       </c>
@@ -930,7 +930,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>12</v>
       </c>
@@ -947,7 +947,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>12</v>
       </c>
@@ -964,7 +964,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>12</v>
       </c>
@@ -981,7 +981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>13</v>
       </c>
@@ -998,12 +998,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>14</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>14</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>14</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>15</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>15</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>15</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>16</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>16</v>
       </c>
@@ -1139,12 +1139,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>17</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>17</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>17</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>18</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>18</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>18</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>19</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>19</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>20</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>20</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>21</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>21</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>21</v>
       </c>
@@ -1359,7 +1359,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>22</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>22</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>22</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>23</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>23</v>
       </c>
@@ -1444,12 +1444,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>23</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>24</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>24</v>
       </c>
@@ -1483,12 +1483,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>25</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>25</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>25</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>26</v>
       </c>
@@ -1550,12 +1550,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>26</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>27</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>27</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>27</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>28</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>28</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>28</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>29</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>29</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>29</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>30</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>30</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>31</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>31</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>31</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>32</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>32</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>32</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>33</v>
       </c>
@@ -1825,12 +1825,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>33</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>33</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>34</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>34</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>34</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>35</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>35</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>35</v>
       </c>
@@ -1943,7 +1943,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>36</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>36</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>36</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>37</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>37</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>38</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>38</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>38</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>39</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>39</v>
       </c>
@@ -2098,12 +2098,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>39</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>40</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>40</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>40</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>41</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>41</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>41</v>
       </c>
@@ -2205,7 +2205,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>42</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>42</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>42</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>43</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>43</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>43</v>
       </c>
@@ -2301,7 +2301,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>44</v>
       </c>
@@ -2318,7 +2318,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>44</v>
       </c>
@@ -2335,12 +2335,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>44</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>45</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>45</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>45</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>46</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>46</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>46</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>47</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>47</v>
       </c>
@@ -2467,7 +2467,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>47</v>
       </c>
@@ -2484,7 +2484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>48</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>48</v>
       </c>
@@ -2518,12 +2518,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>48</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>49</v>
       </c>
@@ -2540,7 +2540,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>49</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>49</v>
       </c>
@@ -2574,7 +2574,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>50</v>
       </c>
@@ -2591,7 +2591,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>50</v>
       </c>
@@ -2608,12 +2608,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>50</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>51</v>
       </c>
@@ -2630,7 +2630,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>51</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>51</v>
       </c>
@@ -2661,7 +2661,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>52</v>
       </c>
@@ -2678,7 +2678,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>52</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>53</v>
       </c>
@@ -2712,7 +2712,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>53</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>53</v>
       </c>
@@ -2746,7 +2746,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>54</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>54</v>
       </c>
@@ -2780,12 +2780,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>54</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>55</v>
       </c>
@@ -2802,7 +2802,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>55</v>
       </c>
@@ -2819,7 +2819,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>55</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>56</v>
       </c>
@@ -2853,7 +2853,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>56</v>
       </c>
@@ -2870,7 +2870,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>56</v>
       </c>
@@ -2878,7 +2878,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>57</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>57</v>
       </c>
@@ -2912,12 +2912,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>57</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>58</v>
       </c>
@@ -2934,7 +2934,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>58</v>
       </c>
@@ -2951,7 +2951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>58</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>59</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>59</v>
       </c>
@@ -3002,7 +3002,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>59</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>60</v>
       </c>
@@ -3036,7 +3036,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>60</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>60</v>
       </c>
@@ -3067,7 +3067,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>61</v>
       </c>
@@ -3084,7 +3084,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>61</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>62</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>62</v>
       </c>
@@ -3132,7 +3132,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>62</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>63</v>
       </c>
@@ -3166,7 +3166,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>63</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>63</v>
       </c>
@@ -3191,7 +3191,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>64</v>
       </c>
@@ -3208,7 +3208,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>64</v>
       </c>
@@ -3225,7 +3225,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>64</v>
       </c>
@@ -3233,7 +3233,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>65</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>65</v>
       </c>
@@ -3267,7 +3267,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>65</v>
       </c>
@@ -3275,7 +3275,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>66</v>
       </c>
@@ -3292,7 +3292,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>66</v>
       </c>
@@ -3309,7 +3309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>66</v>
       </c>
@@ -3326,7 +3326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>67</v>
       </c>
@@ -3343,7 +3343,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>67</v>
       </c>
@@ -3357,7 +3357,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>68</v>
       </c>
@@ -3374,7 +3374,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>68</v>
       </c>
@@ -3391,7 +3391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>68</v>
       </c>
@@ -3405,7 +3405,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>69</v>
       </c>
@@ -3422,7 +3422,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>69</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>69</v>
       </c>
@@ -3456,7 +3456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>70</v>
       </c>
@@ -3473,7 +3473,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>70</v>
       </c>
@@ -3481,12 +3481,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>70</v>
       </c>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>71</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>71</v>
       </c>
@@ -3520,7 +3520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>72</v>
       </c>
@@ -3537,7 +3537,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>72</v>
       </c>
@@ -3554,7 +3554,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>72</v>
       </c>
@@ -3571,7 +3571,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>73</v>
       </c>
@@ -3588,7 +3588,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>73</v>
       </c>
@@ -3605,7 +3605,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>73</v>
       </c>
@@ -3622,7 +3622,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>74</v>
       </c>
@@ -3639,7 +3639,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>74</v>
       </c>
@@ -3656,12 +3656,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>74</v>
       </c>
     </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>75</v>
       </c>
@@ -3678,7 +3678,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>75</v>
       </c>
@@ -3686,7 +3686,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>76</v>
       </c>
@@ -3703,7 +3703,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>76</v>
       </c>
@@ -3720,7 +3720,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>77</v>
       </c>
@@ -3737,7 +3737,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>77</v>
       </c>
@@ -3754,12 +3754,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>77</v>
       </c>
     </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>78</v>
       </c>
@@ -3776,7 +3776,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>78</v>
       </c>
@@ -3793,7 +3793,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>78</v>
       </c>
@@ -3810,7 +3810,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>79</v>
       </c>
@@ -3827,7 +3827,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>79</v>
       </c>
@@ -3844,7 +3844,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>79</v>
       </c>
@@ -3861,7 +3861,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>80</v>
       </c>
@@ -3878,7 +3878,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>80</v>
       </c>
@@ -3895,7 +3895,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>80</v>
       </c>
@@ -3912,7 +3912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>81</v>
       </c>
@@ -3929,7 +3929,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>81</v>
       </c>
@@ -3946,7 +3946,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>81</v>
       </c>
@@ -3963,7 +3963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>82</v>
       </c>
@@ -3980,7 +3980,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>82</v>
       </c>
@@ -3997,7 +3997,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>82</v>
       </c>
@@ -4014,7 +4014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>83</v>
       </c>
@@ -4031,17 +4031,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>83</v>
       </c>
     </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>83</v>
       </c>
     </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>84</v>
       </c>
@@ -4058,7 +4058,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>84</v>
       </c>
@@ -4075,12 +4075,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>84</v>
       </c>
     </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>85</v>
       </c>
@@ -4097,7 +4097,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="236" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>85</v>
       </c>
@@ -4114,7 +4114,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>85</v>
       </c>
@@ -4131,7 +4131,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="238" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>86</v>
       </c>
@@ -4148,7 +4148,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>86</v>
       </c>
@@ -4165,7 +4165,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>86</v>
       </c>
@@ -4182,7 +4182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>87</v>
       </c>
@@ -4199,7 +4199,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>87</v>
       </c>
@@ -4216,7 +4216,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>87</v>
       </c>
@@ -4230,7 +4230,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="244" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>88</v>
       </c>
@@ -4247,7 +4247,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="245" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>88</v>
       </c>
@@ -4264,7 +4264,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>88</v>
       </c>
@@ -4281,7 +4281,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="247" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>89</v>
       </c>
@@ -4298,7 +4298,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>89</v>
       </c>
@@ -4315,7 +4315,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="249" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>89</v>
       </c>
@@ -4329,7 +4329,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="250" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>90</v>
       </c>
@@ -4346,7 +4346,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>90</v>
       </c>
@@ -4363,12 +4363,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="252" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>90</v>
       </c>
     </row>
-    <row r="253" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>91</v>
       </c>
@@ -4385,12 +4385,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="254" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>91</v>
       </c>
     </row>
-    <row r="255" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>92</v>
       </c>
@@ -4407,7 +4407,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="256" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>92</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="257" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>92</v>
       </c>
@@ -4441,7 +4441,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="258" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>93</v>
       </c>
@@ -4458,7 +4458,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="259" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>93</v>
       </c>
@@ -4475,7 +4475,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="260" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>94</v>
       </c>
@@ -4492,7 +4492,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="261" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>94</v>
       </c>
@@ -4509,7 +4509,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="262" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>94</v>
       </c>
@@ -4523,7 +4523,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="263" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>95</v>
       </c>
@@ -4540,7 +4540,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="264" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>95</v>
       </c>
@@ -4557,7 +4557,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="265" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>95</v>
       </c>
@@ -4571,7 +4571,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="266" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>96</v>
       </c>
@@ -4588,7 +4588,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="267" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>96</v>
       </c>
@@ -4596,7 +4596,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="268" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>97</v>
       </c>
@@ -4613,7 +4613,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="269" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>97</v>
       </c>
@@ -4630,12 +4630,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="270" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>97</v>
       </c>
     </row>
-    <row r="271" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>98</v>
       </c>
@@ -4652,7 +4652,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="272" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>98</v>
       </c>
@@ -4669,7 +4669,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>98</v>
       </c>
@@ -4683,7 +4683,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>99</v>
       </c>
@@ -4700,7 +4700,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>99</v>
       </c>
@@ -4717,7 +4717,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>100</v>
       </c>
@@ -4734,7 +4734,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>100</v>
       </c>
@@ -4748,7 +4748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>101</v>
       </c>
@@ -4765,12 +4765,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>101</v>
       </c>
     </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>101</v>
       </c>
@@ -4781,7 +4781,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="281" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>102</v>
       </c>
@@ -4798,12 +4798,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>102</v>
       </c>
     </row>
-    <row r="283" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>103</v>
       </c>
@@ -4820,12 +4820,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="284" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>103</v>
       </c>
     </row>
-    <row r="285" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>104</v>
       </c>
@@ -4842,7 +4842,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="286" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>104</v>
       </c>
@@ -4856,7 +4856,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="287" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>105</v>
       </c>
@@ -4873,7 +4873,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="288" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>105</v>
       </c>
@@ -4890,7 +4890,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>106</v>
       </c>
@@ -4907,12 +4907,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>106</v>
       </c>
     </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>107</v>
       </c>
@@ -4929,7 +4929,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>107</v>
       </c>
@@ -4946,7 +4946,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>108</v>
       </c>
@@ -4963,17 +4963,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>109</v>
       </c>
     </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>109</v>
       </c>
     </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>110</v>
       </c>
@@ -4990,12 +4990,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>110</v>
       </c>
     </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>111</v>
       </c>
@@ -5012,7 +5012,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>112</v>
       </c>
@@ -5029,7 +5029,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>112</v>
       </c>
@@ -5046,7 +5046,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>112</v>
       </c>
@@ -5054,7 +5054,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="302" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>113</v>
       </c>
@@ -5071,7 +5071,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="303" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>113</v>
       </c>
@@ -5088,7 +5088,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="304" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>113</v>
       </c>
@@ -5102,7 +5102,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="305" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>114</v>
       </c>
@@ -5119,7 +5119,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="306" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>114</v>
       </c>
@@ -5136,7 +5136,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="307" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>115</v>
       </c>
@@ -5153,7 +5153,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="308" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>115</v>
       </c>
@@ -5170,7 +5170,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="309" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>116</v>
       </c>
@@ -5187,7 +5187,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="310" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>116</v>
       </c>
@@ -5204,7 +5204,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="311" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>117</v>
       </c>
@@ -5221,7 +5221,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="312" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>117</v>
       </c>
@@ -5238,17 +5238,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="313" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>118</v>
       </c>
     </row>
-    <row r="314" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>118</v>
       </c>
     </row>
-    <row r="315" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>119</v>
       </c>
@@ -5265,12 +5265,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="316" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>119</v>
       </c>
     </row>
-    <row r="317" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>120</v>
       </c>
@@ -5287,17 +5287,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="318" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>120</v>
       </c>
     </row>
-    <row r="319" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>121</v>
       </c>
     </row>
-    <row r="320" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>121</v>
       </c>
@@ -5314,7 +5314,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="321" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>122</v>
       </c>
@@ -5331,7 +5331,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="322" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>122</v>
       </c>
@@ -5348,7 +5348,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="323" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>123</v>
       </c>
@@ -5365,52 +5365,52 @@
         <v>12</v>
       </c>
     </row>
-    <row r="324" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>123</v>
       </c>
     </row>
-    <row r="325" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>124</v>
       </c>
     </row>
-    <row r="326" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>124</v>
       </c>
     </row>
-    <row r="327" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>125</v>
       </c>
     </row>
-    <row r="328" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>125</v>
       </c>
     </row>
-    <row r="329" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>126</v>
       </c>
     </row>
-    <row r="330" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>126</v>
       </c>
     </row>
-    <row r="331" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>127</v>
       </c>
     </row>
-    <row r="332" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>127</v>
       </c>
     </row>
-    <row r="333" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>128</v>
       </c>
@@ -5427,12 +5427,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="334" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>129</v>
       </c>
     </row>
-    <row r="335" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>129</v>
       </c>

</xml_diff>